<commit_message>
- sample name fix
</commit_message>
<xml_diff>
--- a/2024_02 Kelly all samples.xlsx
+++ b/2024_02 Kelly all samples.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE189"/>
+  <dimension ref="A1:AI189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,20 +503,40 @@
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
+          <t>orig.name</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>samplename2</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>newsamplenumber</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>samplename3</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
           <t>order_number</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Konz.(µg/µl)</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>cell_density</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>condition</t>
         </is>
@@ -525,20 +545,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RNA_P2041_S37</t>
+          <t>RNA_P2041_S55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10619_S37_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10752_S55_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RNA_P2041_10619_S37_L003</t>
+          <t>RNA_P2041_10752_S55_L003</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -633,7 +653,25 @@
           <t>RNA_01</t>
         </is>
       </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S37</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S55</t>
+        </is>
+      </c>
+      <c r="AD2">
+        <v>55</v>
+      </c>
       <c r="AE2" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S55</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -642,20 +680,20 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RNA_P2041_S41</t>
+          <t>RNA_P2041_S37</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10632_S41_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10619_S37_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C3">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>RNA_P2041_10632_S41_L003</t>
+          <t>RNA_P2041_10619_S37_L003</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -755,7 +793,25 @@
           <t>RNA_11</t>
         </is>
       </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S41</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S37</t>
+        </is>
+      </c>
+      <c r="AD3">
+        <v>37</v>
+      </c>
       <c r="AE3" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S37</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -764,20 +820,20 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RNA_P2041_S46</t>
+          <t>RNA_P2041_S42</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10640_S46_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10635_S42_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C4">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>RNA_P2041_10640_S46_L003</t>
+          <t>RNA_P2041_10635_S42_L003</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -877,7 +933,25 @@
           <t>RNA_25</t>
         </is>
       </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S46</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S42</t>
+        </is>
+      </c>
+      <c r="AD4">
+        <v>42</v>
+      </c>
       <c r="AE4" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S42</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -989,7 +1063,7 @@
           <t>Katharina_1</t>
         </is>
       </c>
-      <c r="AE5" t="inlineStr">
+      <c r="AI5" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -1101,7 +1175,7 @@
           <t>Katharina_1</t>
         </is>
       </c>
-      <c r="AE6" t="inlineStr">
+      <c r="AI6" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -1213,7 +1287,7 @@
           <t>Katharina_2</t>
         </is>
       </c>
-      <c r="AE7" t="inlineStr">
+      <c r="AI7" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -1325,7 +1399,7 @@
           <t>Katharina_2</t>
         </is>
       </c>
-      <c r="AE8" t="inlineStr">
+      <c r="AI8" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -1430,18 +1504,18 @@
       <c r="X9">
         <v>11691</v>
       </c>
-      <c r="AB9">
+      <c r="AF9">
         <v>53</v>
       </c>
-      <c r="AC9">
+      <c r="AG9">
         <v>0.634133333333333</v>
       </c>
-      <c r="AD9" t="inlineStr">
+      <c r="AH9" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE9" t="inlineStr">
+      <c r="AI9" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -1546,18 +1620,18 @@
       <c r="X10">
         <v>11691</v>
       </c>
-      <c r="AB10">
+      <c r="AF10">
         <v>53</v>
       </c>
-      <c r="AC10">
+      <c r="AG10">
         <v>0.634133333333333</v>
       </c>
-      <c r="AD10" t="inlineStr">
+      <c r="AH10" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE10" t="inlineStr">
+      <c r="AI10" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -1662,18 +1736,18 @@
       <c r="X11">
         <v>11691</v>
       </c>
-      <c r="AB11">
+      <c r="AF11">
         <v>53</v>
       </c>
-      <c r="AC11">
+      <c r="AG11">
         <v>0.634133333333333</v>
       </c>
-      <c r="AD11" t="inlineStr">
+      <c r="AH11" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE11" t="inlineStr">
+      <c r="AI11" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -1778,18 +1852,18 @@
       <c r="X12">
         <v>11692</v>
       </c>
-      <c r="AB12">
+      <c r="AF12">
         <v>54</v>
       </c>
-      <c r="AC12">
+      <c r="AG12">
         <v>0.5348000000000001</v>
       </c>
-      <c r="AD12" t="inlineStr">
+      <c r="AH12" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE12" t="inlineStr">
+      <c r="AI12" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -1894,18 +1968,18 @@
       <c r="X13">
         <v>11692</v>
       </c>
-      <c r="AB13">
+      <c r="AF13">
         <v>54</v>
       </c>
-      <c r="AC13">
+      <c r="AG13">
         <v>0.5348000000000001</v>
       </c>
-      <c r="AD13" t="inlineStr">
+      <c r="AH13" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE13" t="inlineStr">
+      <c r="AI13" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2010,18 +2084,18 @@
       <c r="X14">
         <v>11692</v>
       </c>
-      <c r="AB14">
+      <c r="AF14">
         <v>54</v>
       </c>
-      <c r="AC14">
+      <c r="AG14">
         <v>0.5348000000000001</v>
       </c>
-      <c r="AD14" t="inlineStr">
+      <c r="AH14" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE14" t="inlineStr">
+      <c r="AI14" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2126,18 +2200,18 @@
       <c r="X15">
         <v>11703</v>
       </c>
-      <c r="AB15">
+      <c r="AF15">
         <v>65</v>
       </c>
-      <c r="AC15">
+      <c r="AG15">
         <v>1.1364</v>
       </c>
-      <c r="AD15" t="inlineStr">
+      <c r="AH15" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE15" t="inlineStr">
+      <c r="AI15" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2242,18 +2316,18 @@
       <c r="X16">
         <v>11703</v>
       </c>
-      <c r="AB16">
+      <c r="AF16">
         <v>65</v>
       </c>
-      <c r="AC16">
+      <c r="AG16">
         <v>1.1364</v>
       </c>
-      <c r="AD16" t="inlineStr">
+      <c r="AH16" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE16" t="inlineStr">
+      <c r="AI16" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2358,18 +2432,18 @@
       <c r="X17">
         <v>11703</v>
       </c>
-      <c r="AB17">
+      <c r="AF17">
         <v>65</v>
       </c>
-      <c r="AC17">
+      <c r="AG17">
         <v>1.1364</v>
       </c>
-      <c r="AD17" t="inlineStr">
+      <c r="AH17" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE17" t="inlineStr">
+      <c r="AI17" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2474,18 +2548,18 @@
       <c r="X18">
         <v>11704</v>
       </c>
-      <c r="AB18">
+      <c r="AF18">
         <v>66</v>
       </c>
-      <c r="AC18">
+      <c r="AG18">
         <v>1.1176</v>
       </c>
-      <c r="AD18" t="inlineStr">
+      <c r="AH18" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE18" t="inlineStr">
+      <c r="AI18" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2590,18 +2664,18 @@
       <c r="X19">
         <v>11704</v>
       </c>
-      <c r="AB19">
+      <c r="AF19">
         <v>66</v>
       </c>
-      <c r="AC19">
+      <c r="AG19">
         <v>1.1176</v>
       </c>
-      <c r="AD19" t="inlineStr">
+      <c r="AH19" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE19" t="inlineStr">
+      <c r="AI19" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2706,18 +2780,18 @@
       <c r="X20">
         <v>11704</v>
       </c>
-      <c r="AB20">
+      <c r="AF20">
         <v>66</v>
       </c>
-      <c r="AC20">
+      <c r="AG20">
         <v>1.1176</v>
       </c>
-      <c r="AD20" t="inlineStr">
+      <c r="AH20" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE20" t="inlineStr">
+      <c r="AI20" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2822,18 +2896,18 @@
       <c r="X21">
         <v>11711</v>
       </c>
-      <c r="AB21">
+      <c r="AF21">
         <v>73</v>
       </c>
-      <c r="AC21">
+      <c r="AG21">
         <v>0.7006</v>
       </c>
-      <c r="AD21" t="inlineStr">
+      <c r="AH21" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE21" t="inlineStr">
+      <c r="AI21" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -2938,18 +3012,18 @@
       <c r="X22">
         <v>11711</v>
       </c>
-      <c r="AB22">
+      <c r="AF22">
         <v>73</v>
       </c>
-      <c r="AC22">
+      <c r="AG22">
         <v>0.7006</v>
       </c>
-      <c r="AD22" t="inlineStr">
+      <c r="AH22" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE22" t="inlineStr">
+      <c r="AI22" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3054,18 +3128,18 @@
       <c r="X23">
         <v>11711</v>
       </c>
-      <c r="AB23">
+      <c r="AF23">
         <v>73</v>
       </c>
-      <c r="AC23">
+      <c r="AG23">
         <v>0.7006</v>
       </c>
-      <c r="AD23" t="inlineStr">
+      <c r="AH23" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE23" t="inlineStr">
+      <c r="AI23" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3170,18 +3244,18 @@
       <c r="X24">
         <v>11712</v>
       </c>
-      <c r="AB24">
+      <c r="AF24">
         <v>74</v>
       </c>
-      <c r="AC24">
+      <c r="AG24">
         <v>1.0708</v>
       </c>
-      <c r="AD24" t="inlineStr">
+      <c r="AH24" t="inlineStr">
         <is>
           <t>1:2</t>
         </is>
       </c>
-      <c r="AE24" t="inlineStr">
+      <c r="AI24" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3286,18 +3360,18 @@
       <c r="X25">
         <v>11712</v>
       </c>
-      <c r="AB25">
+      <c r="AF25">
         <v>74</v>
       </c>
-      <c r="AC25">
+      <c r="AG25">
         <v>1.0708</v>
       </c>
-      <c r="AD25" t="inlineStr">
+      <c r="AH25" t="inlineStr">
         <is>
           <t>1:2</t>
         </is>
       </c>
-      <c r="AE25" t="inlineStr">
+      <c r="AI25" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3402,18 +3476,18 @@
       <c r="X26">
         <v>11712</v>
       </c>
-      <c r="AB26">
+      <c r="AF26">
         <v>74</v>
       </c>
-      <c r="AC26">
+      <c r="AG26">
         <v>1.0708</v>
       </c>
-      <c r="AD26" t="inlineStr">
+      <c r="AH26" t="inlineStr">
         <is>
           <t>1:2</t>
         </is>
       </c>
-      <c r="AE26" t="inlineStr">
+      <c r="AI26" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3518,18 +3592,18 @@
       <c r="X27">
         <v>11719</v>
       </c>
-      <c r="AB27">
+      <c r="AF27">
         <v>81</v>
       </c>
-      <c r="AC27">
+      <c r="AG27">
         <v>1.2068</v>
       </c>
-      <c r="AD27" t="inlineStr">
+      <c r="AH27" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE27" t="inlineStr">
+      <c r="AI27" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3634,18 +3708,18 @@
       <c r="X28">
         <v>11719</v>
       </c>
-      <c r="AB28">
+      <c r="AF28">
         <v>81</v>
       </c>
-      <c r="AC28">
+      <c r="AG28">
         <v>1.2068</v>
       </c>
-      <c r="AD28" t="inlineStr">
+      <c r="AH28" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE28" t="inlineStr">
+      <c r="AI28" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3750,18 +3824,18 @@
       <c r="X29">
         <v>11719</v>
       </c>
-      <c r="AB29">
+      <c r="AF29">
         <v>81</v>
       </c>
-      <c r="AC29">
+      <c r="AG29">
         <v>1.2068</v>
       </c>
-      <c r="AD29" t="inlineStr">
+      <c r="AH29" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE29" t="inlineStr">
+      <c r="AI29" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3866,18 +3940,18 @@
       <c r="X30">
         <v>11720</v>
       </c>
-      <c r="AB30">
+      <c r="AF30">
         <v>82</v>
       </c>
-      <c r="AC30">
+      <c r="AG30">
         <v>1.0424</v>
       </c>
-      <c r="AD30" t="inlineStr">
+      <c r="AH30" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE30" t="inlineStr">
+      <c r="AI30" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -3982,18 +4056,18 @@
       <c r="X31">
         <v>11720</v>
       </c>
-      <c r="AB31">
+      <c r="AF31">
         <v>82</v>
       </c>
-      <c r="AC31">
+      <c r="AG31">
         <v>1.0424</v>
       </c>
-      <c r="AD31" t="inlineStr">
+      <c r="AH31" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE31" t="inlineStr">
+      <c r="AI31" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -4098,18 +4172,18 @@
       <c r="X32">
         <v>11720</v>
       </c>
-      <c r="AB32">
+      <c r="AF32">
         <v>82</v>
       </c>
-      <c r="AC32">
+      <c r="AG32">
         <v>1.0424</v>
       </c>
-      <c r="AD32" t="inlineStr">
+      <c r="AH32" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE32" t="inlineStr">
+      <c r="AI32" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -4214,18 +4288,18 @@
       <c r="X33">
         <v>11725</v>
       </c>
-      <c r="AB33">
+      <c r="AF33">
         <v>87</v>
       </c>
-      <c r="AC33">
+      <c r="AG33">
         <v>0.6425999999999999</v>
       </c>
-      <c r="AD33" t="inlineStr">
+      <c r="AH33" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE33" t="inlineStr">
+      <c r="AI33" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -4330,18 +4404,18 @@
       <c r="X34">
         <v>11725</v>
       </c>
-      <c r="AB34">
+      <c r="AF34">
         <v>87</v>
       </c>
-      <c r="AC34">
+      <c r="AG34">
         <v>0.6425999999999999</v>
       </c>
-      <c r="AD34" t="inlineStr">
+      <c r="AH34" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE34" t="inlineStr">
+      <c r="AI34" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -4446,18 +4520,18 @@
       <c r="X35">
         <v>11725</v>
       </c>
-      <c r="AB35">
+      <c r="AF35">
         <v>87</v>
       </c>
-      <c r="AC35">
+      <c r="AG35">
         <v>0.6425999999999999</v>
       </c>
-      <c r="AD35" t="inlineStr">
+      <c r="AH35" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE35" t="inlineStr">
+      <c r="AI35" t="inlineStr">
         <is>
           <t>Kelly_Nx</t>
         </is>
@@ -4466,20 +4540,20 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>RNA_P2041_S42</t>
+          <t>RNA_P2041_S58</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10635_S42_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10755_S58_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C36">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>RNA_P2041_10635_S42_L003</t>
+          <t>RNA_P2041_10755_S58_L003</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -4574,7 +4648,25 @@
           <t>RNA_12</t>
         </is>
       </c>
+      <c r="AB36" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S42</t>
+        </is>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S38</t>
+        </is>
+      </c>
+      <c r="AD36">
+        <v>38</v>
+      </c>
       <c r="AE36" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S58</t>
+        </is>
+      </c>
+      <c r="AI36" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -4583,20 +4675,20 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>RNA_P2041_S47</t>
+          <t>RNA_P2041_S43</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10744_S47_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10636_S43_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C37">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>RNA_P2041_10744_S47_L003</t>
+          <t>RNA_P2041_10636_S43_L003</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -4696,7 +4788,25 @@
           <t>RNA_26</t>
         </is>
       </c>
+      <c r="AB37" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S47</t>
+        </is>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S43</t>
+        </is>
+      </c>
+      <c r="AD37">
+        <v>43</v>
+      </c>
       <c r="AE37" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S43</t>
+        </is>
+      </c>
+      <c r="AI37" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -4808,7 +4918,7 @@
           <t>Katharina_1</t>
         </is>
       </c>
-      <c r="AE38" t="inlineStr">
+      <c r="AI38" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -4920,7 +5030,7 @@
           <t>Katharina_1</t>
         </is>
       </c>
-      <c r="AE39" t="inlineStr">
+      <c r="AI39" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5032,7 +5142,7 @@
           <t>Katharina_2</t>
         </is>
       </c>
-      <c r="AE40" t="inlineStr">
+      <c r="AI40" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5144,7 +5254,7 @@
           <t>Katharina_2</t>
         </is>
       </c>
-      <c r="AE41" t="inlineStr">
+      <c r="AI41" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5249,18 +5359,18 @@
       <c r="X42">
         <v>11697</v>
       </c>
-      <c r="AB42">
+      <c r="AF42">
         <v>59</v>
       </c>
-      <c r="AC42">
+      <c r="AG42">
         <v>0.5322</v>
       </c>
-      <c r="AD42" t="inlineStr">
+      <c r="AH42" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE42" t="inlineStr">
+      <c r="AI42" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5365,18 +5475,18 @@
       <c r="X43">
         <v>11697</v>
       </c>
-      <c r="AB43">
+      <c r="AF43">
         <v>59</v>
       </c>
-      <c r="AC43">
+      <c r="AG43">
         <v>0.5322</v>
       </c>
-      <c r="AD43" t="inlineStr">
+      <c r="AH43" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE43" t="inlineStr">
+      <c r="AI43" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5481,18 +5591,18 @@
       <c r="X44">
         <v>11697</v>
       </c>
-      <c r="AB44">
+      <c r="AF44">
         <v>59</v>
       </c>
-      <c r="AC44">
+      <c r="AG44">
         <v>0.5322</v>
       </c>
-      <c r="AD44" t="inlineStr">
+      <c r="AH44" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE44" t="inlineStr">
+      <c r="AI44" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5597,18 +5707,18 @@
       <c r="X45">
         <v>11698</v>
       </c>
-      <c r="AB45">
+      <c r="AF45">
         <v>60</v>
       </c>
-      <c r="AC45">
+      <c r="AG45">
         <v>0.5182</v>
       </c>
-      <c r="AD45" t="inlineStr">
+      <c r="AH45" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE45" t="inlineStr">
+      <c r="AI45" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5713,18 +5823,18 @@
       <c r="X46">
         <v>11698</v>
       </c>
-      <c r="AB46">
+      <c r="AF46">
         <v>60</v>
       </c>
-      <c r="AC46">
+      <c r="AG46">
         <v>0.5182</v>
       </c>
-      <c r="AD46" t="inlineStr">
+      <c r="AH46" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE46" t="inlineStr">
+      <c r="AI46" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5829,18 +5939,18 @@
       <c r="X47">
         <v>11698</v>
       </c>
-      <c r="AB47">
+      <c r="AF47">
         <v>60</v>
       </c>
-      <c r="AC47">
+      <c r="AG47">
         <v>0.5182</v>
       </c>
-      <c r="AD47" t="inlineStr">
+      <c r="AH47" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE47" t="inlineStr">
+      <c r="AI47" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -5945,18 +6055,18 @@
       <c r="X48">
         <v>11707</v>
       </c>
-      <c r="AB48">
+      <c r="AF48">
         <v>69</v>
       </c>
-      <c r="AC48">
+      <c r="AG48">
         <v>0.9176</v>
       </c>
-      <c r="AD48" t="inlineStr">
+      <c r="AH48" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE48" t="inlineStr">
+      <c r="AI48" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6061,18 +6171,18 @@
       <c r="X49">
         <v>11707</v>
       </c>
-      <c r="AB49">
+      <c r="AF49">
         <v>69</v>
       </c>
-      <c r="AC49">
+      <c r="AG49">
         <v>0.9176</v>
       </c>
-      <c r="AD49" t="inlineStr">
+      <c r="AH49" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE49" t="inlineStr">
+      <c r="AI49" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6177,18 +6287,18 @@
       <c r="X50">
         <v>11707</v>
       </c>
-      <c r="AB50">
+      <c r="AF50">
         <v>69</v>
       </c>
-      <c r="AC50">
+      <c r="AG50">
         <v>0.9176</v>
       </c>
-      <c r="AD50" t="inlineStr">
+      <c r="AH50" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE50" t="inlineStr">
+      <c r="AI50" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6293,18 +6403,18 @@
       <c r="X51">
         <v>11708</v>
       </c>
-      <c r="AB51">
+      <c r="AF51">
         <v>70</v>
       </c>
-      <c r="AC51">
+      <c r="AG51">
         <v>0.9226</v>
       </c>
-      <c r="AD51" t="inlineStr">
+      <c r="AH51" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE51" t="inlineStr">
+      <c r="AI51" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6409,18 +6519,18 @@
       <c r="X52">
         <v>11708</v>
       </c>
-      <c r="AB52">
+      <c r="AF52">
         <v>70</v>
       </c>
-      <c r="AC52">
+      <c r="AG52">
         <v>0.9226</v>
       </c>
-      <c r="AD52" t="inlineStr">
+      <c r="AH52" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE52" t="inlineStr">
+      <c r="AI52" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6525,18 +6635,18 @@
       <c r="X53">
         <v>11708</v>
       </c>
-      <c r="AB53">
+      <c r="AF53">
         <v>70</v>
       </c>
-      <c r="AC53">
+      <c r="AG53">
         <v>0.9226</v>
       </c>
-      <c r="AD53" t="inlineStr">
+      <c r="AH53" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE53" t="inlineStr">
+      <c r="AI53" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6641,18 +6751,18 @@
       <c r="X54">
         <v>11715</v>
       </c>
-      <c r="AB54">
+      <c r="AF54">
         <v>77</v>
       </c>
-      <c r="AC54">
+      <c r="AG54">
         <v>0.5788</v>
       </c>
-      <c r="AD54" t="inlineStr">
+      <c r="AH54" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE54" t="inlineStr">
+      <c r="AI54" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6757,18 +6867,18 @@
       <c r="X55">
         <v>11715</v>
       </c>
-      <c r="AB55">
+      <c r="AF55">
         <v>77</v>
       </c>
-      <c r="AC55">
+      <c r="AG55">
         <v>0.5788</v>
       </c>
-      <c r="AD55" t="inlineStr">
+      <c r="AH55" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE55" t="inlineStr">
+      <c r="AI55" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6873,18 +6983,18 @@
       <c r="X56">
         <v>11715</v>
       </c>
-      <c r="AB56">
+      <c r="AF56">
         <v>77</v>
       </c>
-      <c r="AC56">
+      <c r="AG56">
         <v>0.5788</v>
       </c>
-      <c r="AD56" t="inlineStr">
+      <c r="AH56" t="inlineStr">
         <is>
           <t>1:3</t>
         </is>
       </c>
-      <c r="AE56" t="inlineStr">
+      <c r="AI56" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -6989,18 +7099,18 @@
       <c r="X57">
         <v>11716</v>
       </c>
-      <c r="AB57">
+      <c r="AF57">
         <v>78</v>
       </c>
-      <c r="AC57">
+      <c r="AG57">
         <v>0.8558</v>
       </c>
-      <c r="AD57" t="inlineStr">
+      <c r="AH57" t="inlineStr">
         <is>
           <t>1:2</t>
         </is>
       </c>
-      <c r="AE57" t="inlineStr">
+      <c r="AI57" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -7105,18 +7215,18 @@
       <c r="X58">
         <v>11716</v>
       </c>
-      <c r="AB58">
+      <c r="AF58">
         <v>78</v>
       </c>
-      <c r="AC58">
+      <c r="AG58">
         <v>0.8558</v>
       </c>
-      <c r="AD58" t="inlineStr">
+      <c r="AH58" t="inlineStr">
         <is>
           <t>1:2</t>
         </is>
       </c>
-      <c r="AE58" t="inlineStr">
+      <c r="AI58" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -7221,18 +7331,18 @@
       <c r="X59">
         <v>11716</v>
       </c>
-      <c r="AB59">
+      <c r="AF59">
         <v>78</v>
       </c>
-      <c r="AC59">
+      <c r="AG59">
         <v>0.8558</v>
       </c>
-      <c r="AD59" t="inlineStr">
+      <c r="AH59" t="inlineStr">
         <is>
           <t>1:2</t>
         </is>
       </c>
-      <c r="AE59" t="inlineStr">
+      <c r="AI59" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -7337,18 +7447,18 @@
       <c r="X60">
         <v>11730</v>
       </c>
-      <c r="AB60">
+      <c r="AF60">
         <v>92</v>
       </c>
-      <c r="AC60">
+      <c r="AG60">
         <v>0.961466666666667</v>
       </c>
-      <c r="AD60" t="inlineStr">
+      <c r="AH60" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE60" t="inlineStr">
+      <c r="AI60" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -7453,18 +7563,18 @@
       <c r="X61">
         <v>11730</v>
       </c>
-      <c r="AB61">
+      <c r="AF61">
         <v>92</v>
       </c>
-      <c r="AC61">
+      <c r="AG61">
         <v>0.961466666666667</v>
       </c>
-      <c r="AD61" t="inlineStr">
+      <c r="AH61" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE61" t="inlineStr">
+      <c r="AI61" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -7569,18 +7679,18 @@
       <c r="X62">
         <v>11730</v>
       </c>
-      <c r="AB62">
+      <c r="AF62">
         <v>92</v>
       </c>
-      <c r="AC62">
+      <c r="AG62">
         <v>0.961466666666667</v>
       </c>
-      <c r="AD62" t="inlineStr">
+      <c r="AH62" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE62" t="inlineStr">
+      <c r="AI62" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -7685,18 +7795,18 @@
       <c r="X63">
         <v>11731</v>
       </c>
-      <c r="AB63">
+      <c r="AF63">
         <v>93</v>
       </c>
-      <c r="AC63">
+      <c r="AG63">
         <v>0.8358</v>
       </c>
-      <c r="AD63" t="inlineStr">
+      <c r="AH63" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE63" t="inlineStr">
+      <c r="AI63" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -7801,18 +7911,18 @@
       <c r="X64">
         <v>11731</v>
       </c>
-      <c r="AB64">
+      <c r="AF64">
         <v>93</v>
       </c>
-      <c r="AC64">
+      <c r="AG64">
         <v>0.8358</v>
       </c>
-      <c r="AD64" t="inlineStr">
+      <c r="AH64" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE64" t="inlineStr">
+      <c r="AI64" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -7917,18 +8027,18 @@
       <c r="X65">
         <v>11731</v>
       </c>
-      <c r="AB65">
+      <c r="AF65">
         <v>93</v>
       </c>
-      <c r="AC65">
+      <c r="AG65">
         <v>0.8358</v>
       </c>
-      <c r="AD65" t="inlineStr">
+      <c r="AH65" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE65" t="inlineStr">
+      <c r="AI65" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -8033,18 +8143,18 @@
       <c r="X66">
         <v>11736</v>
       </c>
-      <c r="AB66">
+      <c r="AF66">
         <v>98</v>
       </c>
-      <c r="AC66">
+      <c r="AG66">
         <v>0.38424</v>
       </c>
-      <c r="AD66" t="inlineStr">
+      <c r="AH66" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE66" t="inlineStr">
+      <c r="AI66" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -8149,18 +8259,18 @@
       <c r="X67">
         <v>11736</v>
       </c>
-      <c r="AB67">
+      <c r="AF67">
         <v>98</v>
       </c>
-      <c r="AC67">
+      <c r="AG67">
         <v>0.38424</v>
       </c>
-      <c r="AD67" t="inlineStr">
+      <c r="AH67" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE67" t="inlineStr">
+      <c r="AI67" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -8265,18 +8375,18 @@
       <c r="X68">
         <v>11736</v>
       </c>
-      <c r="AB68">
+      <c r="AF68">
         <v>98</v>
       </c>
-      <c r="AC68">
+      <c r="AG68">
         <v>0.38424</v>
       </c>
-      <c r="AD68" t="inlineStr">
+      <c r="AH68" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE68" t="inlineStr">
+      <c r="AI68" t="inlineStr">
         <is>
           <t>Kelly_Hx</t>
         </is>
@@ -8285,20 +8395,20 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>RNA_P2041_S48</t>
+          <t>RNA_P2041_S44</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10745_S48_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10637_S44_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C69">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>RNA_P2041_10745_S48_L003</t>
+          <t>RNA_P2041_10637_S44_L003</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -8398,7 +8508,25 @@
           <t>RNA_27</t>
         </is>
       </c>
+      <c r="AB69" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S48</t>
+        </is>
+      </c>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S44</t>
+        </is>
+      </c>
+      <c r="AD69">
+        <v>44</v>
+      </c>
       <c r="AE69" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S44</t>
+        </is>
+      </c>
+      <c r="AI69" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -8503,18 +8631,18 @@
       <c r="X70">
         <v>11693</v>
       </c>
-      <c r="AB70">
+      <c r="AF70">
         <v>55</v>
       </c>
-      <c r="AC70">
+      <c r="AG70">
         <v>0.9412</v>
       </c>
-      <c r="AD70" t="inlineStr">
+      <c r="AH70" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE70" t="inlineStr">
+      <c r="AI70" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -8619,18 +8747,18 @@
       <c r="X71">
         <v>11693</v>
       </c>
-      <c r="AB71">
+      <c r="AF71">
         <v>55</v>
       </c>
-      <c r="AC71">
+      <c r="AG71">
         <v>0.9412</v>
       </c>
-      <c r="AD71" t="inlineStr">
+      <c r="AH71" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE71" t="inlineStr">
+      <c r="AI71" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -8735,18 +8863,18 @@
       <c r="X72">
         <v>11693</v>
       </c>
-      <c r="AB72">
+      <c r="AF72">
         <v>55</v>
       </c>
-      <c r="AC72">
+      <c r="AG72">
         <v>0.9412</v>
       </c>
-      <c r="AD72" t="inlineStr">
+      <c r="AH72" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE72" t="inlineStr">
+      <c r="AI72" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -8851,18 +8979,18 @@
       <c r="X73">
         <v>11694</v>
       </c>
-      <c r="AB73">
+      <c r="AF73">
         <v>56</v>
       </c>
-      <c r="AC73">
+      <c r="AG73">
         <v>0.6804</v>
       </c>
-      <c r="AD73" t="inlineStr">
+      <c r="AH73" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE73" t="inlineStr">
+      <c r="AI73" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -8967,18 +9095,18 @@
       <c r="X74">
         <v>11694</v>
       </c>
-      <c r="AB74">
+      <c r="AF74">
         <v>56</v>
       </c>
-      <c r="AC74">
+      <c r="AG74">
         <v>0.6804</v>
       </c>
-      <c r="AD74" t="inlineStr">
+      <c r="AH74" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE74" t="inlineStr">
+      <c r="AI74" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -9083,18 +9211,18 @@
       <c r="X75">
         <v>11694</v>
       </c>
-      <c r="AB75">
+      <c r="AF75">
         <v>56</v>
       </c>
-      <c r="AC75">
+      <c r="AG75">
         <v>0.6804</v>
       </c>
-      <c r="AD75" t="inlineStr">
+      <c r="AH75" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE75" t="inlineStr">
+      <c r="AI75" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -9199,18 +9327,18 @@
       <c r="X76">
         <v>11705</v>
       </c>
-      <c r="AB76">
+      <c r="AF76">
         <v>67</v>
       </c>
-      <c r="AC76">
+      <c r="AG76">
         <v>1.8268</v>
       </c>
-      <c r="AD76" t="inlineStr">
+      <c r="AH76" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE76" t="inlineStr">
+      <c r="AI76" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -9315,18 +9443,18 @@
       <c r="X77">
         <v>11705</v>
       </c>
-      <c r="AB77">
+      <c r="AF77">
         <v>67</v>
       </c>
-      <c r="AC77">
+      <c r="AG77">
         <v>1.8268</v>
       </c>
-      <c r="AD77" t="inlineStr">
+      <c r="AH77" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE77" t="inlineStr">
+      <c r="AI77" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -9431,18 +9559,18 @@
       <c r="X78">
         <v>11705</v>
       </c>
-      <c r="AB78">
+      <c r="AF78">
         <v>67</v>
       </c>
-      <c r="AC78">
+      <c r="AG78">
         <v>1.8268</v>
       </c>
-      <c r="AD78" t="inlineStr">
+      <c r="AH78" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE78" t="inlineStr">
+      <c r="AI78" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -9547,18 +9675,18 @@
       <c r="X79">
         <v>11713</v>
       </c>
-      <c r="AB79">
+      <c r="AF79">
         <v>75</v>
       </c>
-      <c r="AC79">
+      <c r="AG79">
         <v>1.0078</v>
       </c>
-      <c r="AD79" t="inlineStr">
+      <c r="AH79" t="inlineStr">
         <is>
           <t>1:2,5</t>
         </is>
       </c>
-      <c r="AE79" t="inlineStr">
+      <c r="AI79" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -9663,18 +9791,18 @@
       <c r="X80">
         <v>11713</v>
       </c>
-      <c r="AB80">
+      <c r="AF80">
         <v>75</v>
       </c>
-      <c r="AC80">
+      <c r="AG80">
         <v>1.0078</v>
       </c>
-      <c r="AD80" t="inlineStr">
+      <c r="AH80" t="inlineStr">
         <is>
           <t>1:2,5</t>
         </is>
       </c>
-      <c r="AE80" t="inlineStr">
+      <c r="AI80" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -9779,18 +9907,18 @@
       <c r="X81">
         <v>11713</v>
       </c>
-      <c r="AB81">
+      <c r="AF81">
         <v>75</v>
       </c>
-      <c r="AC81">
+      <c r="AG81">
         <v>1.0078</v>
       </c>
-      <c r="AD81" t="inlineStr">
+      <c r="AH81" t="inlineStr">
         <is>
           <t>1:2,5</t>
         </is>
       </c>
-      <c r="AE81" t="inlineStr">
+      <c r="AI81" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -9895,18 +10023,18 @@
       <c r="X82">
         <v>11721</v>
       </c>
-      <c r="AB82">
+      <c r="AF82">
         <v>83</v>
       </c>
-      <c r="AC82">
+      <c r="AG82">
         <v>0.7122000000000001</v>
       </c>
-      <c r="AD82" t="inlineStr">
+      <c r="AH82" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE82" t="inlineStr">
+      <c r="AI82" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10011,18 +10139,18 @@
       <c r="X83">
         <v>11721</v>
       </c>
-      <c r="AB83">
+      <c r="AF83">
         <v>83</v>
       </c>
-      <c r="AC83">
+      <c r="AG83">
         <v>0.7122000000000001</v>
       </c>
-      <c r="AD83" t="inlineStr">
+      <c r="AH83" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE83" t="inlineStr">
+      <c r="AI83" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10127,18 +10255,18 @@
       <c r="X84">
         <v>11721</v>
       </c>
-      <c r="AB84">
+      <c r="AF84">
         <v>83</v>
       </c>
-      <c r="AC84">
+      <c r="AG84">
         <v>0.7122000000000001</v>
       </c>
-      <c r="AD84" t="inlineStr">
+      <c r="AH84" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE84" t="inlineStr">
+      <c r="AI84" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10243,18 +10371,18 @@
       <c r="X85">
         <v>11722</v>
       </c>
-      <c r="AB85">
+      <c r="AF85">
         <v>84</v>
       </c>
-      <c r="AC85">
+      <c r="AG85">
         <v>0.6078</v>
       </c>
-      <c r="AD85" t="inlineStr">
+      <c r="AH85" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE85" t="inlineStr">
+      <c r="AI85" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10359,18 +10487,18 @@
       <c r="X86">
         <v>11722</v>
       </c>
-      <c r="AB86">
+      <c r="AF86">
         <v>84</v>
       </c>
-      <c r="AC86">
+      <c r="AG86">
         <v>0.6078</v>
       </c>
-      <c r="AD86" t="inlineStr">
+      <c r="AH86" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE86" t="inlineStr">
+      <c r="AI86" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10475,18 +10603,18 @@
       <c r="X87">
         <v>11722</v>
       </c>
-      <c r="AB87">
+      <c r="AF87">
         <v>84</v>
       </c>
-      <c r="AC87">
+      <c r="AG87">
         <v>0.6078</v>
       </c>
-      <c r="AD87" t="inlineStr">
+      <c r="AH87" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE87" t="inlineStr">
+      <c r="AI87" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10591,18 +10719,18 @@
       <c r="X88">
         <v>11726</v>
       </c>
-      <c r="AB88">
+      <c r="AF88">
         <v>88</v>
       </c>
-      <c r="AC88">
+      <c r="AG88">
         <v>1.3212</v>
       </c>
-      <c r="AD88" t="inlineStr">
+      <c r="AH88" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE88" t="inlineStr">
+      <c r="AI88" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10707,18 +10835,18 @@
       <c r="X89">
         <v>11726</v>
       </c>
-      <c r="AB89">
+      <c r="AF89">
         <v>88</v>
       </c>
-      <c r="AC89">
+      <c r="AG89">
         <v>1.3212</v>
       </c>
-      <c r="AD89" t="inlineStr">
+      <c r="AH89" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE89" t="inlineStr">
+      <c r="AI89" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10823,18 +10951,18 @@
       <c r="X90">
         <v>11726</v>
       </c>
-      <c r="AB90">
+      <c r="AF90">
         <v>88</v>
       </c>
-      <c r="AC90">
+      <c r="AG90">
         <v>1.3212</v>
       </c>
-      <c r="AD90" t="inlineStr">
+      <c r="AH90" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE90" t="inlineStr">
+      <c r="AI90" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -10939,18 +11067,18 @@
       <c r="X91">
         <v>11727</v>
       </c>
-      <c r="AB91">
+      <c r="AF91">
         <v>89</v>
       </c>
-      <c r="AC91">
+      <c r="AG91">
         <v>1.2904</v>
       </c>
-      <c r="AD91" t="inlineStr">
+      <c r="AH91" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE91" t="inlineStr">
+      <c r="AI91" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -11055,18 +11183,18 @@
       <c r="X92">
         <v>11727</v>
       </c>
-      <c r="AB92">
+      <c r="AF92">
         <v>89</v>
       </c>
-      <c r="AC92">
+      <c r="AG92">
         <v>1.2904</v>
       </c>
-      <c r="AD92" t="inlineStr">
+      <c r="AH92" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE92" t="inlineStr">
+      <c r="AI92" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -11171,18 +11299,18 @@
       <c r="X93">
         <v>11727</v>
       </c>
-      <c r="AB93">
+      <c r="AF93">
         <v>89</v>
       </c>
-      <c r="AC93">
+      <c r="AG93">
         <v>1.2904</v>
       </c>
-      <c r="AD93" t="inlineStr">
+      <c r="AH93" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE93" t="inlineStr">
+      <c r="AI93" t="inlineStr">
         <is>
           <t>HIF1A_Nx</t>
         </is>
@@ -11294,7 +11422,7 @@
           <t>Katharina_1</t>
         </is>
       </c>
-      <c r="AE94" t="inlineStr">
+      <c r="AI94" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -11406,7 +11534,7 @@
           <t>Katharina_1</t>
         </is>
       </c>
-      <c r="AE95" t="inlineStr">
+      <c r="AI95" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -11518,7 +11646,7 @@
           <t>Katharina_2</t>
         </is>
       </c>
-      <c r="AE96" t="inlineStr">
+      <c r="AI96" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -11630,7 +11758,7 @@
           <t>Katharina_2</t>
         </is>
       </c>
-      <c r="AE97" t="inlineStr">
+      <c r="AI97" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -11639,20 +11767,20 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>RNA_P2041_S49</t>
+          <t>RNA_P2041_S45</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10746_S49_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10638_S45_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C98">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>RNA_P2041_10746_S49_L003</t>
+          <t>RNA_P2041_10638_S45_L003</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -11752,7 +11880,25 @@
           <t>RNA_28</t>
         </is>
       </c>
+      <c r="AB98" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S49</t>
+        </is>
+      </c>
+      <c r="AC98" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S45</t>
+        </is>
+      </c>
+      <c r="AD98">
+        <v>45</v>
+      </c>
       <c r="AE98" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S45</t>
+        </is>
+      </c>
+      <c r="AI98" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -11857,18 +12003,18 @@
       <c r="X99">
         <v>11699</v>
       </c>
-      <c r="AB99">
+      <c r="AF99">
         <v>61</v>
       </c>
-      <c r="AC99">
+      <c r="AG99">
         <v>0.7236</v>
       </c>
-      <c r="AD99" t="inlineStr">
+      <c r="AH99" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE99" t="inlineStr">
+      <c r="AI99" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -11973,18 +12119,18 @@
       <c r="X100">
         <v>11699</v>
       </c>
-      <c r="AB100">
+      <c r="AF100">
         <v>61</v>
       </c>
-      <c r="AC100">
+      <c r="AG100">
         <v>0.7236</v>
       </c>
-      <c r="AD100" t="inlineStr">
+      <c r="AH100" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE100" t="inlineStr">
+      <c r="AI100" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -12089,18 +12235,18 @@
       <c r="X101">
         <v>11699</v>
       </c>
-      <c r="AB101">
+      <c r="AF101">
         <v>61</v>
       </c>
-      <c r="AC101">
+      <c r="AG101">
         <v>0.7236</v>
       </c>
-      <c r="AD101" t="inlineStr">
+      <c r="AH101" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE101" t="inlineStr">
+      <c r="AI101" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -12205,18 +12351,18 @@
       <c r="X102">
         <v>11700</v>
       </c>
-      <c r="AB102">
+      <c r="AF102">
         <v>62</v>
       </c>
-      <c r="AC102">
+      <c r="AG102">
         <v>0.6082</v>
       </c>
-      <c r="AD102" t="inlineStr">
+      <c r="AH102" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE102" t="inlineStr">
+      <c r="AI102" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -12321,18 +12467,18 @@
       <c r="X103">
         <v>11700</v>
       </c>
-      <c r="AB103">
+      <c r="AF103">
         <v>62</v>
       </c>
-      <c r="AC103">
+      <c r="AG103">
         <v>0.6082</v>
       </c>
-      <c r="AD103" t="inlineStr">
+      <c r="AH103" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE103" t="inlineStr">
+      <c r="AI103" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -12437,18 +12583,18 @@
       <c r="X104">
         <v>11700</v>
       </c>
-      <c r="AB104">
+      <c r="AF104">
         <v>62</v>
       </c>
-      <c r="AC104">
+      <c r="AG104">
         <v>0.6082</v>
       </c>
-      <c r="AD104" t="inlineStr">
+      <c r="AH104" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE104" t="inlineStr">
+      <c r="AI104" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -12553,18 +12699,18 @@
       <c r="X105">
         <v>11709</v>
       </c>
-      <c r="AB105">
+      <c r="AF105">
         <v>71</v>
       </c>
-      <c r="AC105">
+      <c r="AG105">
         <v>1.0704</v>
       </c>
-      <c r="AD105" t="inlineStr">
+      <c r="AH105" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE105" t="inlineStr">
+      <c r="AI105" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -12669,18 +12815,18 @@
       <c r="X106">
         <v>11709</v>
       </c>
-      <c r="AB106">
+      <c r="AF106">
         <v>71</v>
       </c>
-      <c r="AC106">
+      <c r="AG106">
         <v>1.0704</v>
       </c>
-      <c r="AD106" t="inlineStr">
+      <c r="AH106" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE106" t="inlineStr">
+      <c r="AI106" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -12785,18 +12931,18 @@
       <c r="X107">
         <v>11709</v>
       </c>
-      <c r="AB107">
+      <c r="AF107">
         <v>71</v>
       </c>
-      <c r="AC107">
+      <c r="AG107">
         <v>1.0704</v>
       </c>
-      <c r="AD107" t="inlineStr">
+      <c r="AH107" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE107" t="inlineStr">
+      <c r="AI107" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -12901,18 +13047,18 @@
       <c r="X108">
         <v>11717</v>
       </c>
-      <c r="AB108">
+      <c r="AF108">
         <v>79</v>
       </c>
-      <c r="AC108">
+      <c r="AG108">
         <v>0.895</v>
       </c>
-      <c r="AD108" t="inlineStr">
+      <c r="AH108" t="inlineStr">
         <is>
           <t>1:2,5</t>
         </is>
       </c>
-      <c r="AE108" t="inlineStr">
+      <c r="AI108" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13017,18 +13163,18 @@
       <c r="X109">
         <v>11717</v>
       </c>
-      <c r="AB109">
+      <c r="AF109">
         <v>79</v>
       </c>
-      <c r="AC109">
+      <c r="AG109">
         <v>0.895</v>
       </c>
-      <c r="AD109" t="inlineStr">
+      <c r="AH109" t="inlineStr">
         <is>
           <t>1:2,5</t>
         </is>
       </c>
-      <c r="AE109" t="inlineStr">
+      <c r="AI109" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13133,18 +13279,18 @@
       <c r="X110">
         <v>11717</v>
       </c>
-      <c r="AB110">
+      <c r="AF110">
         <v>79</v>
       </c>
-      <c r="AC110">
+      <c r="AG110">
         <v>0.895</v>
       </c>
-      <c r="AD110" t="inlineStr">
+      <c r="AH110" t="inlineStr">
         <is>
           <t>1:2,5</t>
         </is>
       </c>
-      <c r="AE110" t="inlineStr">
+      <c r="AI110" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13249,18 +13395,18 @@
       <c r="X111">
         <v>11732</v>
       </c>
-      <c r="AB111">
+      <c r="AF111">
         <v>94</v>
       </c>
-      <c r="AC111">
+      <c r="AG111">
         <v>0.4784</v>
       </c>
-      <c r="AD111" t="inlineStr">
+      <c r="AH111" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE111" t="inlineStr">
+      <c r="AI111" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13365,18 +13511,18 @@
       <c r="X112">
         <v>11732</v>
       </c>
-      <c r="AB112">
+      <c r="AF112">
         <v>94</v>
       </c>
-      <c r="AC112">
+      <c r="AG112">
         <v>0.4784</v>
       </c>
-      <c r="AD112" t="inlineStr">
+      <c r="AH112" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE112" t="inlineStr">
+      <c r="AI112" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13481,18 +13627,18 @@
       <c r="X113">
         <v>11732</v>
       </c>
-      <c r="AB113">
+      <c r="AF113">
         <v>94</v>
       </c>
-      <c r="AC113">
+      <c r="AG113">
         <v>0.4784</v>
       </c>
-      <c r="AD113" t="inlineStr">
+      <c r="AH113" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE113" t="inlineStr">
+      <c r="AI113" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13597,18 +13743,18 @@
       <c r="X114">
         <v>11733</v>
       </c>
-      <c r="AB114">
+      <c r="AF114">
         <v>95</v>
       </c>
-      <c r="AC114">
+      <c r="AG114">
         <v>0.5528</v>
       </c>
-      <c r="AD114" t="inlineStr">
+      <c r="AH114" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE114" t="inlineStr">
+      <c r="AI114" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13713,18 +13859,18 @@
       <c r="X115">
         <v>11733</v>
       </c>
-      <c r="AB115">
+      <c r="AF115">
         <v>95</v>
       </c>
-      <c r="AC115">
+      <c r="AG115">
         <v>0.5528</v>
       </c>
-      <c r="AD115" t="inlineStr">
+      <c r="AH115" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE115" t="inlineStr">
+      <c r="AI115" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13829,18 +13975,18 @@
       <c r="X116">
         <v>11733</v>
       </c>
-      <c r="AB116">
+      <c r="AF116">
         <v>95</v>
       </c>
-      <c r="AC116">
+      <c r="AG116">
         <v>0.5528</v>
       </c>
-      <c r="AD116" t="inlineStr">
+      <c r="AH116" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE116" t="inlineStr">
+      <c r="AI116" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -13945,18 +14091,18 @@
       <c r="X117">
         <v>11737</v>
       </c>
-      <c r="AB117">
+      <c r="AF117">
         <v>99</v>
       </c>
-      <c r="AC117">
+      <c r="AG117">
         <v>0.9032</v>
       </c>
-      <c r="AD117" t="inlineStr">
+      <c r="AH117" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE117" t="inlineStr">
+      <c r="AI117" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -14061,18 +14207,18 @@
       <c r="X118">
         <v>11737</v>
       </c>
-      <c r="AB118">
+      <c r="AF118">
         <v>99</v>
       </c>
-      <c r="AC118">
+      <c r="AG118">
         <v>0.9032</v>
       </c>
-      <c r="AD118" t="inlineStr">
+      <c r="AH118" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE118" t="inlineStr">
+      <c r="AI118" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -14177,18 +14323,18 @@
       <c r="X119">
         <v>11737</v>
       </c>
-      <c r="AB119">
+      <c r="AF119">
         <v>99</v>
       </c>
-      <c r="AC119">
+      <c r="AG119">
         <v>0.9032</v>
       </c>
-      <c r="AD119" t="inlineStr">
+      <c r="AH119" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE119" t="inlineStr">
+      <c r="AI119" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -14293,18 +14439,18 @@
       <c r="X120">
         <v>11738</v>
       </c>
-      <c r="AB120">
+      <c r="AF120">
         <v>100</v>
       </c>
-      <c r="AC120">
+      <c r="AG120">
         <v>0.9468</v>
       </c>
-      <c r="AD120" t="inlineStr">
+      <c r="AH120" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE120" t="inlineStr">
+      <c r="AI120" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -14409,18 +14555,18 @@
       <c r="X121">
         <v>11738</v>
       </c>
-      <c r="AB121">
+      <c r="AF121">
         <v>100</v>
       </c>
-      <c r="AC121">
+      <c r="AG121">
         <v>0.9468</v>
       </c>
-      <c r="AD121" t="inlineStr">
+      <c r="AH121" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE121" t="inlineStr">
+      <c r="AI121" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -14525,18 +14671,18 @@
       <c r="X122">
         <v>11738</v>
       </c>
-      <c r="AB122">
+      <c r="AF122">
         <v>100</v>
       </c>
-      <c r="AC122">
+      <c r="AG122">
         <v>0.9468</v>
       </c>
-      <c r="AD122" t="inlineStr">
+      <c r="AH122" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE122" t="inlineStr">
+      <c r="AI122" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -14545,20 +14691,20 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>RNA_P2041_S50</t>
+          <t>RNA_P2041_S46</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10747_S50_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10640_S46_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C123">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>RNA_P2041_10747_S50_L003</t>
+          <t>RNA_P2041_10640_S46_L003</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -14658,7 +14804,25 @@
           <t>RNA_30</t>
         </is>
       </c>
+      <c r="AB123" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S50</t>
+        </is>
+      </c>
+      <c r="AC123" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S46</t>
+        </is>
+      </c>
+      <c r="AD123">
+        <v>46</v>
+      </c>
       <c r="AE123" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S46</t>
+        </is>
+      </c>
+      <c r="AI123" t="inlineStr">
         <is>
           <t>HIF1A_Hx</t>
         </is>
@@ -14763,18 +14927,18 @@
       <c r="X124">
         <v>11695</v>
       </c>
-      <c r="AB124">
+      <c r="AF124">
         <v>57</v>
       </c>
-      <c r="AC124">
+      <c r="AG124">
         <v>1.6428</v>
       </c>
-      <c r="AD124" t="inlineStr">
+      <c r="AH124" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE124" t="inlineStr">
+      <c r="AI124" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -14879,18 +15043,18 @@
       <c r="X125">
         <v>11695</v>
       </c>
-      <c r="AB125">
+      <c r="AF125">
         <v>57</v>
       </c>
-      <c r="AC125">
+      <c r="AG125">
         <v>1.6428</v>
       </c>
-      <c r="AD125" t="inlineStr">
+      <c r="AH125" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE125" t="inlineStr">
+      <c r="AI125" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -14995,18 +15159,18 @@
       <c r="X126">
         <v>11695</v>
       </c>
-      <c r="AB126">
+      <c r="AF126">
         <v>57</v>
       </c>
-      <c r="AC126">
+      <c r="AG126">
         <v>1.6428</v>
       </c>
-      <c r="AD126" t="inlineStr">
+      <c r="AH126" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE126" t="inlineStr">
+      <c r="AI126" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -15111,18 +15275,18 @@
       <c r="X127">
         <v>11696</v>
       </c>
-      <c r="AB127">
+      <c r="AF127">
         <v>58</v>
       </c>
-      <c r="AC127">
+      <c r="AG127">
         <v>1.0744</v>
       </c>
-      <c r="AD127" t="inlineStr">
+      <c r="AH127" t="inlineStr">
         <is>
           <t>1:6</t>
         </is>
       </c>
-      <c r="AE127" t="inlineStr">
+      <c r="AI127" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -15227,18 +15391,18 @@
       <c r="X128">
         <v>11696</v>
       </c>
-      <c r="AB128">
+      <c r="AF128">
         <v>58</v>
       </c>
-      <c r="AC128">
+      <c r="AG128">
         <v>1.0744</v>
       </c>
-      <c r="AD128" t="inlineStr">
+      <c r="AH128" t="inlineStr">
         <is>
           <t>1:6</t>
         </is>
       </c>
-      <c r="AE128" t="inlineStr">
+      <c r="AI128" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -15343,18 +15507,18 @@
       <c r="X129">
         <v>11696</v>
       </c>
-      <c r="AB129">
+      <c r="AF129">
         <v>58</v>
       </c>
-      <c r="AC129">
+      <c r="AG129">
         <v>1.0744</v>
       </c>
-      <c r="AD129" t="inlineStr">
+      <c r="AH129" t="inlineStr">
         <is>
           <t>1:6</t>
         </is>
       </c>
-      <c r="AE129" t="inlineStr">
+      <c r="AI129" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -15459,18 +15623,18 @@
       <c r="X130">
         <v>11706</v>
       </c>
-      <c r="AB130">
+      <c r="AF130">
         <v>68</v>
       </c>
-      <c r="AC130">
+      <c r="AG130">
         <v>1.4206</v>
       </c>
-      <c r="AD130" t="inlineStr">
+      <c r="AH130" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE130" t="inlineStr">
+      <c r="AI130" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -15575,18 +15739,18 @@
       <c r="X131">
         <v>11706</v>
       </c>
-      <c r="AB131">
+      <c r="AF131">
         <v>68</v>
       </c>
-      <c r="AC131">
+      <c r="AG131">
         <v>1.4206</v>
       </c>
-      <c r="AD131" t="inlineStr">
+      <c r="AH131" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE131" t="inlineStr">
+      <c r="AI131" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -15691,18 +15855,18 @@
       <c r="X132">
         <v>11706</v>
       </c>
-      <c r="AB132">
+      <c r="AF132">
         <v>68</v>
       </c>
-      <c r="AC132">
+      <c r="AG132">
         <v>1.4206</v>
       </c>
-      <c r="AD132" t="inlineStr">
+      <c r="AH132" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE132" t="inlineStr">
+      <c r="AI132" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -15807,18 +15971,18 @@
       <c r="X133">
         <v>11714</v>
       </c>
-      <c r="AB133">
+      <c r="AF133">
         <v>76</v>
       </c>
-      <c r="AC133">
+      <c r="AG133">
         <v>0.36788</v>
       </c>
-      <c r="AD133" t="inlineStr">
+      <c r="AH133" t="inlineStr">
         <is>
           <t>1:1,5</t>
         </is>
       </c>
-      <c r="AE133" t="inlineStr">
+      <c r="AI133" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -15923,18 +16087,18 @@
       <c r="X134">
         <v>11714</v>
       </c>
-      <c r="AB134">
+      <c r="AF134">
         <v>76</v>
       </c>
-      <c r="AC134">
+      <c r="AG134">
         <v>0.36788</v>
       </c>
-      <c r="AD134" t="inlineStr">
+      <c r="AH134" t="inlineStr">
         <is>
           <t>1:1,5</t>
         </is>
       </c>
-      <c r="AE134" t="inlineStr">
+      <c r="AI134" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16039,18 +16203,18 @@
       <c r="X135">
         <v>11714</v>
       </c>
-      <c r="AB135">
+      <c r="AF135">
         <v>76</v>
       </c>
-      <c r="AC135">
+      <c r="AG135">
         <v>0.36788</v>
       </c>
-      <c r="AD135" t="inlineStr">
+      <c r="AH135" t="inlineStr">
         <is>
           <t>1:1,5</t>
         </is>
       </c>
-      <c r="AE135" t="inlineStr">
+      <c r="AI135" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16155,18 +16319,18 @@
       <c r="X136">
         <v>11723</v>
       </c>
-      <c r="AB136">
+      <c r="AF136">
         <v>85</v>
       </c>
-      <c r="AC136">
+      <c r="AG136">
         <v>0.9514</v>
       </c>
-      <c r="AD136" t="inlineStr">
+      <c r="AH136" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE136" t="inlineStr">
+      <c r="AI136" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16271,18 +16435,18 @@
       <c r="X137">
         <v>11723</v>
       </c>
-      <c r="AB137">
+      <c r="AF137">
         <v>85</v>
       </c>
-      <c r="AC137">
+      <c r="AG137">
         <v>0.9514</v>
       </c>
-      <c r="AD137" t="inlineStr">
+      <c r="AH137" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE137" t="inlineStr">
+      <c r="AI137" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16387,18 +16551,18 @@
       <c r="X138">
         <v>11723</v>
       </c>
-      <c r="AB138">
+      <c r="AF138">
         <v>85</v>
       </c>
-      <c r="AC138">
+      <c r="AG138">
         <v>0.9514</v>
       </c>
-      <c r="AD138" t="inlineStr">
+      <c r="AH138" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE138" t="inlineStr">
+      <c r="AI138" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16503,18 +16667,18 @@
       <c r="X139">
         <v>11724</v>
       </c>
-      <c r="AB139">
+      <c r="AF139">
         <v>86</v>
       </c>
-      <c r="AC139">
+      <c r="AG139">
         <v>1.0252</v>
       </c>
-      <c r="AD139" t="inlineStr">
+      <c r="AH139" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE139" t="inlineStr">
+      <c r="AI139" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16619,18 +16783,18 @@
       <c r="X140">
         <v>11724</v>
       </c>
-      <c r="AB140">
+      <c r="AF140">
         <v>86</v>
       </c>
-      <c r="AC140">
+      <c r="AG140">
         <v>1.0252</v>
       </c>
-      <c r="AD140" t="inlineStr">
+      <c r="AH140" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE140" t="inlineStr">
+      <c r="AI140" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16735,18 +16899,18 @@
       <c r="X141">
         <v>11724</v>
       </c>
-      <c r="AB141">
+      <c r="AF141">
         <v>86</v>
       </c>
-      <c r="AC141">
+      <c r="AG141">
         <v>1.0252</v>
       </c>
-      <c r="AD141" t="inlineStr">
+      <c r="AH141" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE141" t="inlineStr">
+      <c r="AI141" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16851,18 +17015,18 @@
       <c r="X142">
         <v>11728</v>
       </c>
-      <c r="AB142">
+      <c r="AF142">
         <v>90</v>
       </c>
-      <c r="AC142">
+      <c r="AG142">
         <v>1.6632</v>
       </c>
-      <c r="AD142" t="inlineStr">
+      <c r="AH142" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE142" t="inlineStr">
+      <c r="AI142" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -16967,18 +17131,18 @@
       <c r="X143">
         <v>11728</v>
       </c>
-      <c r="AB143">
+      <c r="AF143">
         <v>90</v>
       </c>
-      <c r="AC143">
+      <c r="AG143">
         <v>1.6632</v>
       </c>
-      <c r="AD143" t="inlineStr">
+      <c r="AH143" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE143" t="inlineStr">
+      <c r="AI143" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -17083,18 +17247,18 @@
       <c r="X144">
         <v>11728</v>
       </c>
-      <c r="AB144">
+      <c r="AF144">
         <v>90</v>
       </c>
-      <c r="AC144">
+      <c r="AG144">
         <v>1.6632</v>
       </c>
-      <c r="AD144" t="inlineStr">
+      <c r="AH144" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE144" t="inlineStr">
+      <c r="AI144" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -17199,18 +17363,18 @@
       <c r="X145">
         <v>11729</v>
       </c>
-      <c r="AB145">
+      <c r="AF145">
         <v>91</v>
       </c>
-      <c r="AC145">
+      <c r="AG145">
         <v>1.6054</v>
       </c>
-      <c r="AD145" t="inlineStr">
+      <c r="AH145" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE145" t="inlineStr">
+      <c r="AI145" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -17315,18 +17479,18 @@
       <c r="X146">
         <v>11729</v>
       </c>
-      <c r="AB146">
+      <c r="AF146">
         <v>91</v>
       </c>
-      <c r="AC146">
+      <c r="AG146">
         <v>1.6054</v>
       </c>
-      <c r="AD146" t="inlineStr">
+      <c r="AH146" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE146" t="inlineStr">
+      <c r="AI146" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -17431,18 +17595,18 @@
       <c r="X147">
         <v>11729</v>
       </c>
-      <c r="AB147">
+      <c r="AF147">
         <v>91</v>
       </c>
-      <c r="AC147">
+      <c r="AG147">
         <v>1.6054</v>
       </c>
-      <c r="AD147" t="inlineStr">
+      <c r="AH147" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE147" t="inlineStr">
+      <c r="AI147" t="inlineStr">
         <is>
           <t>HIF2A_Nx</t>
         </is>
@@ -17554,7 +17718,7 @@
           <t>Katharina_1</t>
         </is>
       </c>
-      <c r="AE148" t="inlineStr">
+      <c r="AI148" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -17666,7 +17830,7 @@
           <t>Katharina_1</t>
         </is>
       </c>
-      <c r="AE149" t="inlineStr">
+      <c r="AI149" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -17778,7 +17942,7 @@
           <t>Katharina_2</t>
         </is>
       </c>
-      <c r="AE150" t="inlineStr">
+      <c r="AI150" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -17890,7 +18054,7 @@
           <t>Katharina_2</t>
         </is>
       </c>
-      <c r="AE151" t="inlineStr">
+      <c r="AI151" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -17995,18 +18159,18 @@
       <c r="X152">
         <v>11701</v>
       </c>
-      <c r="AB152">
+      <c r="AF152">
         <v>63</v>
       </c>
-      <c r="AC152">
+      <c r="AG152">
         <v>0.9692</v>
       </c>
-      <c r="AD152" t="inlineStr">
+      <c r="AH152" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE152" t="inlineStr">
+      <c r="AI152" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -18111,18 +18275,18 @@
       <c r="X153">
         <v>11701</v>
       </c>
-      <c r="AB153">
+      <c r="AF153">
         <v>63</v>
       </c>
-      <c r="AC153">
+      <c r="AG153">
         <v>0.9692</v>
       </c>
-      <c r="AD153" t="inlineStr">
+      <c r="AH153" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE153" t="inlineStr">
+      <c r="AI153" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -18227,18 +18391,18 @@
       <c r="X154">
         <v>11701</v>
       </c>
-      <c r="AB154">
+      <c r="AF154">
         <v>63</v>
       </c>
-      <c r="AC154">
+      <c r="AG154">
         <v>0.9692</v>
       </c>
-      <c r="AD154" t="inlineStr">
+      <c r="AH154" t="inlineStr">
         <is>
           <t>1:5</t>
         </is>
       </c>
-      <c r="AE154" t="inlineStr">
+      <c r="AI154" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -18343,18 +18507,18 @@
       <c r="X155">
         <v>11702</v>
       </c>
-      <c r="AB155">
+      <c r="AF155">
         <v>64</v>
       </c>
-      <c r="AC155">
+      <c r="AG155">
         <v>0.7742</v>
       </c>
-      <c r="AD155" t="inlineStr">
+      <c r="AH155" t="inlineStr">
         <is>
           <t>1:6</t>
         </is>
       </c>
-      <c r="AE155" t="inlineStr">
+      <c r="AI155" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -18459,18 +18623,18 @@
       <c r="X156">
         <v>11702</v>
       </c>
-      <c r="AB156">
+      <c r="AF156">
         <v>64</v>
       </c>
-      <c r="AC156">
+      <c r="AG156">
         <v>0.7742</v>
       </c>
-      <c r="AD156" t="inlineStr">
+      <c r="AH156" t="inlineStr">
         <is>
           <t>1:6</t>
         </is>
       </c>
-      <c r="AE156" t="inlineStr">
+      <c r="AI156" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -18575,18 +18739,18 @@
       <c r="X157">
         <v>11702</v>
       </c>
-      <c r="AB157">
+      <c r="AF157">
         <v>64</v>
       </c>
-      <c r="AC157">
+      <c r="AG157">
         <v>0.7742</v>
       </c>
-      <c r="AD157" t="inlineStr">
+      <c r="AH157" t="inlineStr">
         <is>
           <t>1:6</t>
         </is>
       </c>
-      <c r="AE157" t="inlineStr">
+      <c r="AI157" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -18691,18 +18855,18 @@
       <c r="X158">
         <v>11710</v>
       </c>
-      <c r="AB158">
+      <c r="AF158">
         <v>72</v>
       </c>
-      <c r="AC158">
+      <c r="AG158">
         <v>1.0128</v>
       </c>
-      <c r="AD158" t="inlineStr">
+      <c r="AH158" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE158" t="inlineStr">
+      <c r="AI158" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -18807,18 +18971,18 @@
       <c r="X159">
         <v>11710</v>
       </c>
-      <c r="AB159">
+      <c r="AF159">
         <v>72</v>
       </c>
-      <c r="AC159">
+      <c r="AG159">
         <v>1.0128</v>
       </c>
-      <c r="AD159" t="inlineStr">
+      <c r="AH159" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE159" t="inlineStr">
+      <c r="AI159" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -18923,18 +19087,18 @@
       <c r="X160">
         <v>11710</v>
       </c>
-      <c r="AB160">
+      <c r="AF160">
         <v>72</v>
       </c>
-      <c r="AC160">
+      <c r="AG160">
         <v>1.0128</v>
       </c>
-      <c r="AD160" t="inlineStr">
+      <c r="AH160" t="inlineStr">
         <is>
           <t>1:4</t>
         </is>
       </c>
-      <c r="AE160" t="inlineStr">
+      <c r="AI160" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19039,18 +19203,18 @@
       <c r="X161">
         <v>11718</v>
       </c>
-      <c r="AB161">
+      <c r="AF161">
         <v>80</v>
       </c>
-      <c r="AC161">
+      <c r="AG161">
         <v>0.37856</v>
       </c>
-      <c r="AD161" t="inlineStr">
+      <c r="AH161" t="inlineStr">
         <is>
           <t>1:1,5</t>
         </is>
       </c>
-      <c r="AE161" t="inlineStr">
+      <c r="AI161" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19155,18 +19319,18 @@
       <c r="X162">
         <v>11718</v>
       </c>
-      <c r="AB162">
+      <c r="AF162">
         <v>80</v>
       </c>
-      <c r="AC162">
+      <c r="AG162">
         <v>0.37856</v>
       </c>
-      <c r="AD162" t="inlineStr">
+      <c r="AH162" t="inlineStr">
         <is>
           <t>1:1,5</t>
         </is>
       </c>
-      <c r="AE162" t="inlineStr">
+      <c r="AI162" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19271,18 +19435,18 @@
       <c r="X163">
         <v>11718</v>
       </c>
-      <c r="AB163">
+      <c r="AF163">
         <v>80</v>
       </c>
-      <c r="AC163">
+      <c r="AG163">
         <v>0.37856</v>
       </c>
-      <c r="AD163" t="inlineStr">
+      <c r="AH163" t="inlineStr">
         <is>
           <t>1:1,5</t>
         </is>
       </c>
-      <c r="AE163" t="inlineStr">
+      <c r="AI163" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19387,18 +19551,18 @@
       <c r="X164">
         <v>11734</v>
       </c>
-      <c r="AB164">
+      <c r="AF164">
         <v>96</v>
       </c>
-      <c r="AC164">
+      <c r="AG164">
         <v>0.8372000000000001</v>
       </c>
-      <c r="AD164" t="inlineStr">
+      <c r="AH164" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE164" t="inlineStr">
+      <c r="AI164" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19503,18 +19667,18 @@
       <c r="X165">
         <v>11734</v>
       </c>
-      <c r="AB165">
+      <c r="AF165">
         <v>96</v>
       </c>
-      <c r="AC165">
+      <c r="AG165">
         <v>0.8372000000000001</v>
       </c>
-      <c r="AD165" t="inlineStr">
+      <c r="AH165" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE165" t="inlineStr">
+      <c r="AI165" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19619,18 +19783,18 @@
       <c r="X166">
         <v>11734</v>
       </c>
-      <c r="AB166">
+      <c r="AF166">
         <v>96</v>
       </c>
-      <c r="AC166">
+      <c r="AG166">
         <v>0.8372000000000001</v>
       </c>
-      <c r="AD166" t="inlineStr">
+      <c r="AH166" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE166" t="inlineStr">
+      <c r="AI166" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19735,18 +19899,18 @@
       <c r="X167">
         <v>11735</v>
       </c>
-      <c r="AB167">
+      <c r="AF167">
         <v>97</v>
       </c>
-      <c r="AC167">
+      <c r="AG167">
         <v>0.7554</v>
       </c>
-      <c r="AD167" t="inlineStr">
+      <c r="AH167" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE167" t="inlineStr">
+      <c r="AI167" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19851,18 +20015,18 @@
       <c r="X168">
         <v>11735</v>
       </c>
-      <c r="AB168">
+      <c r="AF168">
         <v>97</v>
       </c>
-      <c r="AC168">
+      <c r="AG168">
         <v>0.7554</v>
       </c>
-      <c r="AD168" t="inlineStr">
+      <c r="AH168" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE168" t="inlineStr">
+      <c r="AI168" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -19967,18 +20131,18 @@
       <c r="X169">
         <v>11735</v>
       </c>
-      <c r="AB169">
+      <c r="AF169">
         <v>97</v>
       </c>
-      <c r="AC169">
+      <c r="AG169">
         <v>0.7554</v>
       </c>
-      <c r="AD169" t="inlineStr">
+      <c r="AH169" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="AE169" t="inlineStr">
+      <c r="AI169" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -20083,18 +20247,18 @@
       <c r="X170">
         <v>11739</v>
       </c>
-      <c r="AB170">
+      <c r="AF170">
         <v>101</v>
       </c>
-      <c r="AC170">
+      <c r="AG170">
         <v>1.2554</v>
       </c>
-      <c r="AD170" t="inlineStr">
+      <c r="AH170" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE170" t="inlineStr">
+      <c r="AI170" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -20199,18 +20363,18 @@
       <c r="X171">
         <v>11739</v>
       </c>
-      <c r="AB171">
+      <c r="AF171">
         <v>101</v>
       </c>
-      <c r="AC171">
+      <c r="AG171">
         <v>1.2554</v>
       </c>
-      <c r="AD171" t="inlineStr">
+      <c r="AH171" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE171" t="inlineStr">
+      <c r="AI171" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -20315,18 +20479,18 @@
       <c r="X172">
         <v>11739</v>
       </c>
-      <c r="AB172">
+      <c r="AF172">
         <v>101</v>
       </c>
-      <c r="AC172">
+      <c r="AG172">
         <v>1.2554</v>
       </c>
-      <c r="AD172" t="inlineStr">
+      <c r="AH172" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE172" t="inlineStr">
+      <c r="AI172" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -20431,18 +20595,18 @@
       <c r="X173">
         <v>11740</v>
       </c>
-      <c r="AB173">
+      <c r="AF173">
         <v>102</v>
       </c>
-      <c r="AC173">
+      <c r="AG173">
         <v>1.344</v>
       </c>
-      <c r="AD173" t="inlineStr">
+      <c r="AH173" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE173" t="inlineStr">
+      <c r="AI173" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -20547,18 +20711,18 @@
       <c r="X174">
         <v>11740</v>
       </c>
-      <c r="AB174">
+      <c r="AF174">
         <v>102</v>
       </c>
-      <c r="AC174">
+      <c r="AG174">
         <v>1.344</v>
       </c>
-      <c r="AD174" t="inlineStr">
+      <c r="AH174" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE174" t="inlineStr">
+      <c r="AI174" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -20663,18 +20827,18 @@
       <c r="X175">
         <v>11740</v>
       </c>
-      <c r="AB175">
+      <c r="AF175">
         <v>102</v>
       </c>
-      <c r="AC175">
+      <c r="AG175">
         <v>1.344</v>
       </c>
-      <c r="AD175" t="inlineStr">
+      <c r="AH175" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="AE175" t="inlineStr">
+      <c r="AI175" t="inlineStr">
         <is>
           <t>HIF2A_Hx</t>
         </is>
@@ -20683,20 +20847,20 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>RNA_P2041_S57</t>
+          <t>RNA_P2041_S53</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10754_S57_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10750_S53_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C176">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>RNA_P2041_10754_S57_L003</t>
+          <t>RNA_P2041_10750_S53_L003</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -20786,7 +20950,25 @@
           <t>RNA_39</t>
         </is>
       </c>
+      <c r="AB176" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S57</t>
+        </is>
+      </c>
+      <c r="AC176" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S53</t>
+        </is>
+      </c>
+      <c r="AD176">
+        <v>53</v>
+      </c>
       <c r="AE176" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S53</t>
+        </is>
+      </c>
+      <c r="AI176" t="inlineStr">
         <is>
           <t>HIF1B_Nx</t>
         </is>
@@ -20795,20 +20977,20 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>RNA_P2041_S40</t>
+          <t>RNA_P2041_S38</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10631_S40_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10621_S38_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C177">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>RNA_P2041_10631_S40_L003</t>
+          <t>RNA_P2041_10621_S38_L003</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -20898,7 +21080,25 @@
           <t>RNA_05</t>
         </is>
       </c>
+      <c r="AB177" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S40</t>
+        </is>
+      </c>
+      <c r="AC177" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S58</t>
+        </is>
+      </c>
+      <c r="AD177">
+        <v>58</v>
+      </c>
       <c r="AE177" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S38</t>
+        </is>
+      </c>
+      <c r="AI177" t="inlineStr">
         <is>
           <t>HIF1B_Nx</t>
         </is>
@@ -20907,20 +21107,20 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>RNA_P2041_S44</t>
+          <t>RNA_P2041_S40</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10637_S44_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10631_S40_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C178">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>RNA_P2041_10637_S44_L003</t>
+          <t>RNA_P2041_10631_S40_L003</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -21020,7 +21220,25 @@
           <t>RNA_21</t>
         </is>
       </c>
+      <c r="AB178" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S44</t>
+        </is>
+      </c>
+      <c r="AC178" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S40</t>
+        </is>
+      </c>
+      <c r="AD178">
+        <v>40</v>
+      </c>
       <c r="AE178" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S40</t>
+        </is>
+      </c>
+      <c r="AI178" t="inlineStr">
         <is>
           <t>HIF1B_Nx</t>
         </is>
@@ -21029,20 +21247,20 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>RNA_P2041_S43</t>
+          <t>RNA_P2041_S39</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10636_S43_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10625_S39_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C179">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>RNA_P2041_10636_S43_L003</t>
+          <t>RNA_P2041_10625_S39_L003</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -21132,7 +21350,25 @@
           <t>RNA_15</t>
         </is>
       </c>
+      <c r="AB179" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S43</t>
+        </is>
+      </c>
+      <c r="AC179" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S39</t>
+        </is>
+      </c>
+      <c r="AD179">
+        <v>39</v>
+      </c>
       <c r="AE179" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S39</t>
+        </is>
+      </c>
+      <c r="AI179" t="inlineStr">
         <is>
           <t>HIF1B_Nx</t>
         </is>
@@ -21141,20 +21377,20 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>RNA_P2041_S51</t>
+          <t>RNA_P2041_S48</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10748_S51_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10745_S48_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C180">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>RNA_P2041_10748_S51_L003</t>
+          <t>RNA_P2041_10745_S48_L003</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -21249,7 +21485,25 @@
           <t>RNA_33</t>
         </is>
       </c>
+      <c r="AB180" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S51</t>
+        </is>
+      </c>
+      <c r="AC180" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S47</t>
+        </is>
+      </c>
+      <c r="AD180">
+        <v>47</v>
+      </c>
       <c r="AE180" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S48</t>
+        </is>
+      </c>
+      <c r="AI180" t="inlineStr">
         <is>
           <t>HIF1B_Nx</t>
         </is>
@@ -21258,20 +21512,20 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>RNA_P2041_S53</t>
+          <t>RNA_P2041_S49</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10750_S53_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10746_S49_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C181">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>RNA_P2041_10750_S53_L003</t>
+          <t>RNA_P2041_10746_S49_L003</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -21361,7 +21615,25 @@
           <t>RNA_35</t>
         </is>
       </c>
+      <c r="AB181" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S53</t>
+        </is>
+      </c>
+      <c r="AC181" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S49</t>
+        </is>
+      </c>
+      <c r="AD181">
+        <v>49</v>
+      </c>
       <c r="AE181" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S49</t>
+        </is>
+      </c>
+      <c r="AI181" t="inlineStr">
         <is>
           <t>HIF1B_Nx</t>
         </is>
@@ -21370,20 +21642,20 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>RNA_P2041_S38</t>
+          <t>RNA_P2041_S57</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10621_S38_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10754_S57_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C182">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>RNA_P2041_10621_S38_L003</t>
+          <t>RNA_P2041_10754_S57_L003</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -21483,7 +21755,25 @@
           <t>RNA_03</t>
         </is>
       </c>
+      <c r="AB182" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S38</t>
+        </is>
+      </c>
+      <c r="AC182" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S56</t>
+        </is>
+      </c>
+      <c r="AD182">
+        <v>56</v>
+      </c>
       <c r="AE182" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S57</t>
+        </is>
+      </c>
+      <c r="AI182" t="inlineStr">
         <is>
           <t>HIF1B_Nx</t>
         </is>
@@ -21492,20 +21782,20 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>RNA_P2041_S55</t>
+          <t>RNA_P2041_S51</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10752_S55_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10748_S51_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C183">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>RNA_P2041_10752_S55_L003</t>
+          <t>RNA_P2041_10748_S51_L003</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -21595,7 +21885,25 @@
           <t>RNA_37</t>
         </is>
       </c>
+      <c r="AB183" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S55</t>
+        </is>
+      </c>
+      <c r="AC183" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S51</t>
+        </is>
+      </c>
+      <c r="AD183">
+        <v>51</v>
+      </c>
       <c r="AE183" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S51</t>
+        </is>
+      </c>
+      <c r="AI183" t="inlineStr">
         <is>
           <t>HIF1B_Nx</t>
         </is>
@@ -21604,20 +21912,20 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>RNA_P2041_S58</t>
+          <t>RNA_P2041_S54</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10755_S58_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10751_S54_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C184">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>RNA_P2041_10755_S58_L003</t>
+          <t>RNA_P2041_10751_S54_L003</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -21707,7 +22015,25 @@
           <t>RNA_40</t>
         </is>
       </c>
+      <c r="AB184" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S58</t>
+        </is>
+      </c>
+      <c r="AC184" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S54</t>
+        </is>
+      </c>
+      <c r="AD184">
+        <v>54</v>
+      </c>
       <c r="AE184" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S54</t>
+        </is>
+      </c>
+      <c r="AI184" t="inlineStr">
         <is>
           <t>HIF1B_Hx</t>
         </is>
@@ -21716,20 +22042,20 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>RNA_P2041_S45</t>
+          <t>RNA_P2041_S41</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10638_S45_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10632_S41_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C185">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>RNA_P2041_10638_S45_L003</t>
+          <t>RNA_P2041_10632_S41_L003</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -21824,7 +22150,25 @@
           <t>RNA_22</t>
         </is>
       </c>
+      <c r="AB185" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S45</t>
+        </is>
+      </c>
+      <c r="AC185" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S41</t>
+        </is>
+      </c>
+      <c r="AD185">
+        <v>41</v>
+      </c>
       <c r="AE185" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S41</t>
+        </is>
+      </c>
+      <c r="AI185" t="inlineStr">
         <is>
           <t>HIF1B_Hx</t>
         </is>
@@ -21833,20 +22177,20 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>RNA_P2041_S52</t>
+          <t>RNA_P2041_S47</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10749_S52_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10744_S47_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C186">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>RNA_P2041_10749_S52_L003</t>
+          <t>RNA_P2041_10744_S47_L003</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -21936,7 +22280,25 @@
           <t>RNA_34</t>
         </is>
       </c>
+      <c r="AB186" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S52</t>
+        </is>
+      </c>
+      <c r="AC186" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S48</t>
+        </is>
+      </c>
+      <c r="AD186">
+        <v>48</v>
+      </c>
       <c r="AE186" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S47</t>
+        </is>
+      </c>
+      <c r="AI186" t="inlineStr">
         <is>
           <t>HIF1B_Hx</t>
         </is>
@@ -21945,20 +22307,20 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>RNA_P2041_S54</t>
+          <t>RNA_P2041_S50</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10751_S54_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10747_S50_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C187">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>RNA_P2041_10751_S54_L003</t>
+          <t>RNA_P2041_10747_S50_L003</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -22048,7 +22410,25 @@
           <t>RNA_36</t>
         </is>
       </c>
+      <c r="AB187" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S54</t>
+        </is>
+      </c>
+      <c r="AC187" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S50</t>
+        </is>
+      </c>
+      <c r="AD187">
+        <v>50</v>
+      </c>
       <c r="AE187" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S50</t>
+        </is>
+      </c>
+      <c r="AI187" t="inlineStr">
         <is>
           <t>HIF1B_Hx</t>
         </is>
@@ -22057,20 +22437,20 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>RNA_P2041_S39</t>
+          <t>RNA_P2041_S56</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10625_S39_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10753_S56_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C188">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>RNA_P2041_10625_S39_L003</t>
+          <t>RNA_P2041_10753_S56_L003</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -22170,7 +22550,25 @@
           <t>RNA_04</t>
         </is>
       </c>
+      <c r="AB188" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S39</t>
+        </is>
+      </c>
+      <c r="AC188" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S57</t>
+        </is>
+      </c>
+      <c r="AD188">
+        <v>57</v>
+      </c>
       <c r="AE188" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S56</t>
+        </is>
+      </c>
+      <c r="AI188" t="inlineStr">
         <is>
           <t>HIF1B_Hx</t>
         </is>
@@ -22179,20 +22577,20 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>RNA_P2041_S56</t>
+          <t>RNA_P2041_S52</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10753_S56_L003_quant/quant.sf</t>
+          <t>/mnt/s/AG/AG-Scholz-NGS/Daten/Simon/RNA-Seq_Kelly_all/quants/P2041_10749_S52_L003_quant/quant.sf</t>
         </is>
       </c>
       <c r="C189">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>RNA_P2041_10753_S56_L003</t>
+          <t>RNA_P2041_10749_S52_L003</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -22282,7 +22680,25 @@
           <t>RNA_38</t>
         </is>
       </c>
+      <c r="AB189" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S56</t>
+        </is>
+      </c>
+      <c r="AC189" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S52</t>
+        </is>
+      </c>
+      <c r="AD189">
+        <v>52</v>
+      </c>
       <c r="AE189" t="inlineStr">
+        <is>
+          <t>RNA_P2041_S52</t>
+        </is>
+      </c>
+      <c r="AI189" t="inlineStr">
         <is>
           <t>HIF1B_Hx</t>
         </is>

</xml_diff>